<commit_message>
Week 3 Stat Corrections
</commit_message>
<xml_diff>
--- a/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
+++ b/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Contestant Points" sheetId="4" r:id="rId1"/>
@@ -729,15 +729,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="9.5546875" customWidth="1"/>
+    <col min="2" max="7" width="9.5546875" customWidth="1"/>
     <col min="8" max="8" width="30.109375" customWidth="1"/>
     <col min="9" max="9" width="5.109375" customWidth="1"/>
     <col min="10" max="10" width="36.44140625" customWidth="1"/>
@@ -870,7 +869,7 @@
         <v>70</v>
       </c>
       <c r="T2">
-        <f>SUM(Q2:S2)</f>
+        <f t="shared" ref="T2:T32" si="0">SUM(Q2:S2)</f>
         <v>105</v>
       </c>
     </row>
@@ -900,22 +899,22 @@
         <v>1</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I32" si="0">H3/SUM($H$2:$H$32)</f>
+        <f t="shared" ref="I3:I32" si="1">H3/SUM($H$2:$H$32)</f>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J32" si="1">CONCATENATE(ROUND(I3*100,0),"% of people have chosen this contestant")</f>
+        <f t="shared" ref="J3:J32" si="2">CONCATENATE(ROUND(I3*100,0),"% of people have chosen this contestant")</f>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" s="2">
-        <f t="shared" ref="O3:O32" si="2">N3/SUM($N$2:$N$32)</f>
+        <f t="shared" ref="O3:O32" si="3">N3/SUM($N$2:$N$32)</f>
         <v>0.02</v>
       </c>
       <c r="P3" s="2" t="str">
-        <f t="shared" ref="P3:P32" si="3">CONCATENATE(ROUND(O3*100,0),"% of people have chosen this contestant")</f>
+        <f t="shared" ref="P3:P32" si="4">CONCATENATE(ROUND(O3*100,0),"% of people have chosen this contestant")</f>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q3">
@@ -928,7 +927,7 @@
         <v>100</v>
       </c>
       <c r="T3">
-        <f>SUM(Q3:S3)</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
@@ -958,22 +957,22 @@
         <v>3</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="J4" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7% of people have chosen this contestant</v>
       </c>
       <c r="N4">
         <v>2</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="P4" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q4">
@@ -983,11 +982,11 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="T4">
-        <f>SUM(Q4:S4)</f>
-        <v>110</v>
+        <f t="shared" si="0"/>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -1016,22 +1015,22 @@
         <v>0</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J5" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P5" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q5">
@@ -1044,7 +1043,7 @@
         <v>15</v>
       </c>
       <c r="T5">
-        <f>SUM(Q5:S5)</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
@@ -1074,22 +1073,22 @@
         <v>2</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="N6">
         <v>6</v>
       </c>
       <c r="O6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="P6" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12% of people have chosen this contestant</v>
       </c>
       <c r="Q6">
@@ -1102,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <f>SUM(Q6:S6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1132,22 +1131,22 @@
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J7" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P7" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q7">
@@ -1160,7 +1159,7 @@
         <v>75</v>
       </c>
       <c r="T7">
-        <f>SUM(Q7:S7)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -1190,22 +1189,22 @@
         <v>5</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="J8" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11% of people have chosen this contestant</v>
       </c>
       <c r="N8">
         <v>4</v>
       </c>
       <c r="O8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
       <c r="P8" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8% of people have chosen this contestant</v>
       </c>
       <c r="Q8">
@@ -1218,7 +1217,7 @@
         <v>65</v>
       </c>
       <c r="T8">
-        <f>SUM(Q8:S8)</f>
+        <f t="shared" si="0"/>
         <v>125</v>
       </c>
     </row>
@@ -1248,22 +1247,22 @@
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J9" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="P9" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q9">
@@ -1276,7 +1275,7 @@
         <v>75</v>
       </c>
       <c r="T9">
-        <f>SUM(Q9:S9)</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
@@ -1306,22 +1305,22 @@
         <v>1</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J10" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N10">
         <v>2</v>
       </c>
       <c r="O10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="P10" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q10">
@@ -1331,11 +1330,11 @@
         <v>55</v>
       </c>
       <c r="S10">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="T10">
-        <f>SUM(Q10:S10)</f>
-        <v>130</v>
+        <f t="shared" si="0"/>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -1364,22 +1363,22 @@
         <v>5</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="J11" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11% of people have chosen this contestant</v>
       </c>
       <c r="N11">
         <v>7</v>
       </c>
       <c r="O11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="P11" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14% of people have chosen this contestant</v>
       </c>
       <c r="Q11">
@@ -1392,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="T11">
-        <f>SUM(Q11:S11)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
@@ -1422,22 +1421,22 @@
         <v>6</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13333333333333333</v>
       </c>
       <c r="J12" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13% of people have chosen this contestant</v>
       </c>
       <c r="N12">
         <v>2</v>
       </c>
       <c r="O12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="P12" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q12">
@@ -1450,7 +1449,7 @@
         <v>45</v>
       </c>
       <c r="T12">
-        <f>SUM(Q12:S12)</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
@@ -1480,22 +1479,22 @@
         <v>3</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="J13" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7% of people have chosen this contestant</v>
       </c>
       <c r="N13">
         <v>2</v>
       </c>
       <c r="O13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="P13" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q13">
@@ -1508,7 +1507,7 @@
         <v>105</v>
       </c>
       <c r="T13">
-        <f>SUM(Q13:S13)</f>
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
     </row>
@@ -1538,22 +1537,22 @@
         <v>0</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J14" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="P14" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q14">
@@ -1566,7 +1565,7 @@
         <v>65</v>
       </c>
       <c r="T14">
-        <f>SUM(Q14:S14)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -1596,22 +1595,22 @@
         <v>0</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J15" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P15" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q15">
@@ -1624,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <f>SUM(Q15:S15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1654,22 +1653,22 @@
         <v>0</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J16" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P16" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q16">
@@ -1682,7 +1681,7 @@
         <v>60</v>
       </c>
       <c r="T16">
-        <f>SUM(Q16:S16)</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
@@ -1712,22 +1711,22 @@
         <v>1</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N17">
         <v>3</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
       <c r="P17" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q17">
@@ -1740,7 +1739,7 @@
         <v>70</v>
       </c>
       <c r="T17">
-        <f>SUM(Q17:S17)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
@@ -1770,22 +1769,22 @@
         <v>1</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P18" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q18">
@@ -1798,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <f>SUM(Q18:S18)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
@@ -1828,22 +1827,22 @@
         <v>1</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N19">
         <v>3</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
       <c r="P19" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q19">
@@ -1856,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <f>SUM(Q19:S19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1886,22 +1885,22 @@
         <v>0</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J20" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P20" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q20">
@@ -1914,7 +1913,7 @@
         <v>55</v>
       </c>
       <c r="T20">
-        <f>SUM(Q20:S20)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
     </row>
@@ -1944,22 +1943,22 @@
         <v>1</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J21" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N21">
         <v>2</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="P21" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q21">
@@ -1972,7 +1971,7 @@
         <v>15</v>
       </c>
       <c r="T21">
-        <f>SUM(Q21:S21)</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
@@ -2002,22 +2001,22 @@
         <v>3</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="J22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7% of people have chosen this contestant</v>
       </c>
       <c r="N22">
         <v>1</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="P22" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q22">
@@ -2030,7 +2029,7 @@
         <v>80</v>
       </c>
       <c r="T22">
-        <f>SUM(Q22:S22)</f>
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
     </row>
@@ -2060,22 +2059,22 @@
         <v>1</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
       <c r="O23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P23" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q23">
@@ -2088,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="T23">
-        <f>SUM(Q23:S23)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2118,22 +2117,22 @@
         <v>1</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P24" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q24">
@@ -2146,7 +2145,7 @@
         <v>90</v>
       </c>
       <c r="T24">
-        <f>SUM(Q24:S24)</f>
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
     </row>
@@ -2176,22 +2175,22 @@
         <v>0</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J25" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P25" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q25">
@@ -2204,7 +2203,7 @@
         <v>35</v>
       </c>
       <c r="T25">
-        <f>SUM(Q25:S25)</f>
+        <f t="shared" si="0"/>
         <v>135</v>
       </c>
     </row>
@@ -2234,22 +2233,22 @@
         <v>1</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J26" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N26">
         <v>2</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
       <c r="P26" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q26">
@@ -2262,7 +2261,7 @@
         <v>40</v>
       </c>
       <c r="T26">
-        <f>SUM(Q26:S26)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
     </row>
@@ -2292,22 +2291,22 @@
         <v>2</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="J27" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="N27">
         <v>3</v>
       </c>
       <c r="O27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
       <c r="P27" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q27">
@@ -2320,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="T27">
-        <f>SUM(Q27:S27)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2350,22 +2349,22 @@
         <v>0</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J28" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N28">
         <v>0</v>
       </c>
       <c r="O28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P28" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q28">
@@ -2378,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="T28">
-        <f>SUM(Q28:S28)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -2408,22 +2407,22 @@
         <v>1</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J29" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="N29">
         <v>0</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P29" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q29">
@@ -2436,7 +2435,7 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <f>SUM(Q29:S29)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -2466,22 +2465,22 @@
         <v>4</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.8888888888888892E-2</v>
       </c>
       <c r="J30" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9% of people have chosen this contestant</v>
       </c>
       <c r="N30">
         <v>1</v>
       </c>
       <c r="O30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="P30" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q30">
@@ -2494,7 +2493,7 @@
         <v>40</v>
       </c>
       <c r="T30">
-        <f>SUM(Q30:S30)</f>
+        <f t="shared" si="0"/>
         <v>145</v>
       </c>
     </row>
@@ -2524,22 +2523,22 @@
         <v>0</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J31" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N31">
         <v>3</v>
       </c>
       <c r="O31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
       <c r="P31" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q31">
@@ -2552,7 +2551,7 @@
         <v>0</v>
       </c>
       <c r="T31">
-        <f>SUM(Q31:S31)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2582,22 +2581,22 @@
         <v>2</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="J32" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="N32">
         <v>3</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.06</v>
       </c>
       <c r="P32" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q32">
@@ -2610,7 +2609,7 @@
         <v>65</v>
       </c>
       <c r="T32">
-        <f>SUM(Q32:S32)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -2935,11 +2934,11 @@
       </c>
       <c r="F7">
         <f>VLOOKUP(B7,'Contestant Points'!$A$2:$S$32,19,FALSE)</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="H7" t="str">
         <f>VLOOKUP(B7,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -3559,11 +3558,11 @@
       </c>
       <c r="F20">
         <f>VLOOKUP(B20,'Contestant Points'!$A$2:$S$32,19,FALSE)</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="H20" t="str">
         <f>VLOOKUP(B20,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4039,11 +4038,11 @@
       </c>
       <c r="F30">
         <f>VLOOKUP(B30,'Contestant Points'!$A$2:$S$32,19,FALSE)</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H30" t="str">
         <f>VLOOKUP(B30,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4375,11 +4374,11 @@
       </c>
       <c r="F37">
         <f>VLOOKUP(B37,'Contestant Points'!$A$2:$S$32,19,FALSE)</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="H37" t="str">
         <f>VLOOKUP(B37,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4954,11 +4953,11 @@
       </c>
       <c r="F4">
         <f>VLOOKUP(B4,'Contestant Points'!$A$2:$S$32,19,FALSE)</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -5122,11 +5121,11 @@
       </c>
       <c r="F10">
         <f>VLOOKUP(B10,'Contestant Points'!$A$2:$S$32,19,FALSE)</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -5446,8 +5445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5997,11 +5996,11 @@
       </c>
       <c r="F12">
         <f>VLOOKUP(B12,'Contestant Points'!$A$2:$T$32,19,FALSE)</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="H12" t="str">
         <f>VLOOKUP(B12,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -6045,11 +6044,11 @@
       </c>
       <c r="F13">
         <f>VLOOKUP(B13,'Contestant Points'!$A$2:$T$32,19,FALSE)</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H13" t="str">
         <f>VLOOKUP(B13,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -6477,11 +6476,11 @@
       </c>
       <c r="F22">
         <f>VLOOKUP(B22,'Contestant Points'!$A$2:$T$32,19,FALSE)</f>
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="H22" t="str">
         <f>VLOOKUP(B22,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -7677,11 +7676,11 @@
       </c>
       <c r="F47">
         <f>VLOOKUP(B47,'Contestant Points'!$A$2:$T$32,19,FALSE)</f>
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G47">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H47" t="str">
         <f>VLOOKUP(B47,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>

</xml_diff>

<commit_message>
Added in 13 Pine Street Dashboard
</commit_message>
<xml_diff>
--- a/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
+++ b/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contestant Points" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="120">
   <si>
     <t>Team</t>
   </si>
@@ -729,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,6 +844,13 @@
         <f>CONCATENATE(ROUND(I2*100,0),"% of people have chosen this contestant")</f>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <f>K2/SUM($K$2:$K$32)</f>
+        <v>0</v>
+      </c>
       <c r="M2" s="2" t="str">
         <f>CONCATENATE(ROUND(L2*100,0),"% of people have chosen this contestant")</f>
         <v>0% of people have chosen this contestant</v>
@@ -906,15 +913,26 @@
         <f t="shared" ref="J3:J32" si="2">CONCATENATE(ROUND(I3*100,0),"% of people have chosen this contestant")</f>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" ref="L3:L32" si="3">K3/SUM($K$2:$K$32)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="str">
+        <f t="shared" ref="M3:M32" si="4">CONCATENATE(ROUND(L3*100,0),"% of people have chosen this contestant")</f>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" s="2">
-        <f t="shared" ref="O3:O32" si="3">N3/SUM($N$2:$N$32)</f>
+        <f t="shared" ref="O3:O32" si="5">N3/SUM($N$2:$N$32)</f>
         <v>0.02</v>
       </c>
       <c r="P3" s="2" t="str">
-        <f t="shared" ref="P3:P32" si="4">CONCATENATE(ROUND(O3*100,0),"% of people have chosen this contestant")</f>
+        <f t="shared" ref="P3:P32" si="6">CONCATENATE(ROUND(O3*100,0),"% of people have chosen this contestant")</f>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q3">
@@ -964,15 +982,26 @@
         <f t="shared" si="2"/>
         <v>7% of people have chosen this contestant</v>
       </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>10% of people have chosen this contestant</v>
+      </c>
       <c r="N4">
         <v>2</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P4" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q4">
@@ -1022,15 +1051,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P5" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q5">
@@ -1080,15 +1120,26 @@
         <f t="shared" si="2"/>
         <v>4% of people have chosen this contestant</v>
       </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N6">
         <v>6</v>
       </c>
       <c r="O6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.12</v>
       </c>
       <c r="P6" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12% of people have chosen this contestant</v>
       </c>
       <c r="Q6">
@@ -1138,15 +1189,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q7">
@@ -1196,15 +1258,26 @@
         <f t="shared" si="2"/>
         <v>11% of people have chosen this contestant</v>
       </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="M8" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>15% of people have chosen this contestant</v>
+      </c>
       <c r="N8">
         <v>4</v>
       </c>
       <c r="O8" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.08</v>
       </c>
       <c r="P8" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8% of people have chosen this contestant</v>
       </c>
       <c r="Q8">
@@ -1254,15 +1327,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="P9" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q9">
@@ -1312,15 +1396,26 @@
         <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N10">
         <v>2</v>
       </c>
       <c r="O10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P10" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q10">
@@ -1370,15 +1465,26 @@
         <f t="shared" si="2"/>
         <v>11% of people have chosen this contestant</v>
       </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="M11" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>15% of people have chosen this contestant</v>
+      </c>
       <c r="N11">
         <v>7</v>
       </c>
       <c r="O11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="P11" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14% of people have chosen this contestant</v>
       </c>
       <c r="Q11">
@@ -1428,15 +1534,26 @@
         <f t="shared" si="2"/>
         <v>13% of people have chosen this contestant</v>
       </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="M12" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>5% of people have chosen this contestant</v>
+      </c>
       <c r="N12">
         <v>2</v>
       </c>
       <c r="O12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P12" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q12">
@@ -1486,15 +1603,26 @@
         <f t="shared" si="2"/>
         <v>7% of people have chosen this contestant</v>
       </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="M13" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>5% of people have chosen this contestant</v>
+      </c>
       <c r="N13">
         <v>2</v>
       </c>
       <c r="O13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P13" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q13">
@@ -1544,15 +1672,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="M14" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>5% of people have chosen this contestant</v>
+      </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="P14" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q14">
@@ -1602,15 +1741,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P15" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q15">
@@ -1660,15 +1810,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P16" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q16">
@@ -1718,15 +1879,26 @@
         <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="M17" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>20% of people have chosen this contestant</v>
+      </c>
       <c r="N17">
         <v>3</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P17" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q17">
@@ -1776,15 +1948,26 @@
         <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P18" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q18">
@@ -1834,15 +2017,26 @@
         <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N19">
         <v>3</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P19" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q19">
@@ -1892,15 +2086,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P20" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q20">
@@ -1950,15 +2155,26 @@
         <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="M21" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>10% of people have chosen this contestant</v>
+      </c>
       <c r="N21">
         <v>2</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P21" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q21">
@@ -2008,15 +2224,26 @@
         <f t="shared" si="2"/>
         <v>7% of people have chosen this contestant</v>
       </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="M22" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>5% of people have chosen this contestant</v>
+      </c>
       <c r="N22">
         <v>1</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="P22" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q22">
@@ -2066,15 +2293,26 @@
         <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N23">
         <v>0</v>
       </c>
       <c r="O23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P23" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q23">
@@ -2124,15 +2362,26 @@
         <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P24" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q24">
@@ -2182,15 +2431,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P25" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q25">
@@ -2240,15 +2500,26 @@
         <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N26">
         <v>2</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P26" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q26">
@@ -2298,15 +2569,26 @@
         <f t="shared" si="2"/>
         <v>4% of people have chosen this contestant</v>
       </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N27">
         <v>3</v>
       </c>
       <c r="O27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P27" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q27">
@@ -2356,15 +2638,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N28">
         <v>0</v>
       </c>
       <c r="O28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P28" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q28">
@@ -2414,15 +2707,26 @@
         <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N29">
         <v>0</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P29" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q29">
@@ -2472,15 +2776,26 @@
         <f t="shared" si="2"/>
         <v>9% of people have chosen this contestant</v>
       </c>
+      <c r="K30">
+        <v>2</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="M30" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>10% of people have chosen this contestant</v>
+      </c>
       <c r="N30">
         <v>1</v>
       </c>
       <c r="O30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="P30" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q30">
@@ -2530,15 +2845,26 @@
         <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N31">
         <v>3</v>
       </c>
       <c r="O31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P31" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q31">
@@ -2588,15 +2914,26 @@
         <f t="shared" si="2"/>
         <v>4% of people have chosen this contestant</v>
       </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0% of people have chosen this contestant</v>
+      </c>
       <c r="N32">
         <v>3</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P32" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q32">
@@ -2623,7 +2960,7 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4841,9 +5178,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4853,7 +5192,7 @@
     <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4875,8 +5214,23 @@
       <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -4903,8 +5257,28 @@
         <f>SUM(D2:F2)</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="str">
+        <f>VLOOKUP(B2,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>0% of people have chosen this contestant</v>
+      </c>
+      <c r="I2">
+        <f>VLOOKUP(B2,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="J2" t="str">
+        <f>VLOOKUP(B2,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Executive Assistant</v>
+      </c>
+      <c r="K2" t="str">
+        <f>VLOOKUP(B2,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'</v>
+      </c>
+      <c r="L2" t="str">
+        <f>VLOOKUP(B2,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4931,8 +5305,28 @@
         <f t="shared" ref="G3:G21" si="0">SUM(D3:F3)</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="str">
+        <f>VLOOKUP(B3,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>13% of people have chosen this contestant</v>
+      </c>
+      <c r="I3">
+        <f>VLOOKUP(B3,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="J3" t="str">
+        <f>VLOOKUP(B3,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Senior Inventory Analyst</v>
+      </c>
+      <c r="K3" t="str">
+        <f>VLOOKUP(B3,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>5'11"</v>
+      </c>
+      <c r="L3" t="str">
+        <f>VLOOKUP(B3,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -4959,8 +5353,28 @@
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="str">
+        <f>VLOOKUP(B4,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>7% of people have chosen this contestant</v>
+      </c>
+      <c r="I4">
+        <f>VLOOKUP(B4,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="J4" t="str">
+        <f>VLOOKUP(B4,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Education Software Manager</v>
+      </c>
+      <c r="K4" t="str">
+        <f>VLOOKUP(B4,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'3"</v>
+      </c>
+      <c r="L4" t="str">
+        <f>VLOOKUP(B4,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -4987,8 +5401,28 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="str">
+        <f>VLOOKUP(B5,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>2% of people have chosen this contestant</v>
+      </c>
+      <c r="I5">
+        <f>VLOOKUP(B5,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="J5" t="str">
+        <f>VLOOKUP(B5,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Attorney</v>
+      </c>
+      <c r="K5" t="str">
+        <f>VLOOKUP(B5,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>5'11"</v>
+      </c>
+      <c r="L5" t="str">
+        <f>VLOOKUP(B5,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>Caucasian</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -5015,8 +5449,28 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="str">
+        <f>VLOOKUP(B6,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>2% of people have chosen this contestant</v>
+      </c>
+      <c r="I6">
+        <f>VLOOKUP(B6,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="J6" t="str">
+        <f>VLOOKUP(B6,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Attorney</v>
+      </c>
+      <c r="K6" t="str">
+        <f>VLOOKUP(B6,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>5'11"</v>
+      </c>
+      <c r="L6" t="str">
+        <f>VLOOKUP(B6,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>Caucasian</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -5043,8 +5497,28 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="str">
+        <f>VLOOKUP(B7,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>11% of people have chosen this contestant</v>
+      </c>
+      <c r="I7">
+        <f>VLOOKUP(B7,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="J7" t="str">
+        <f>VLOOKUP(B7,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Chiropractor</v>
+      </c>
+      <c r="K7" t="str">
+        <f>VLOOKUP(B7,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'2"</v>
+      </c>
+      <c r="L7" t="str">
+        <f>VLOOKUP(B7,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>Caucasian</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -5071,8 +5545,28 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="str">
+        <f>VLOOKUP(B8,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>11% of people have chosen this contestant</v>
+      </c>
+      <c r="I8">
+        <f>VLOOKUP(B8,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="J8" t="str">
+        <f>VLOOKUP(B8,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Executive Recruiter</v>
+      </c>
+      <c r="K8" t="str">
+        <f>VLOOKUP(B8,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'4"</v>
+      </c>
+      <c r="L8" t="str">
+        <f>VLOOKUP(B8,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -5099,8 +5593,28 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="str">
+        <f>VLOOKUP(B9,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>2% of people have chosen this contestant</v>
+      </c>
+      <c r="I9">
+        <f>VLOOKUP(B9,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="J9" t="str">
+        <f>VLOOKUP(B9,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Prosecuting Attorney</v>
+      </c>
+      <c r="K9" t="str">
+        <f>VLOOKUP(B9,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'3"</v>
+      </c>
+      <c r="L9" t="str">
+        <f>VLOOKUP(B9,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -5127,8 +5641,28 @@
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="str">
+        <f>VLOOKUP(B10,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>7% of people have chosen this contestant</v>
+      </c>
+      <c r="I10">
+        <f>VLOOKUP(B10,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="J10" t="str">
+        <f>VLOOKUP(B10,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Education Software Manager</v>
+      </c>
+      <c r="K10" t="str">
+        <f>VLOOKUP(B10,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'3"</v>
+      </c>
+      <c r="L10" t="str">
+        <f>VLOOKUP(B10,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -5155,8 +5689,28 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="str">
+        <f>VLOOKUP(B11,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>11% of people have chosen this contestant</v>
+      </c>
+      <c r="I11">
+        <f>VLOOKUP(B11,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="J11" t="str">
+        <f>VLOOKUP(B11,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Chiropractor</v>
+      </c>
+      <c r="K11" t="str">
+        <f>VLOOKUP(B11,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'2"</v>
+      </c>
+      <c r="L11" t="str">
+        <f>VLOOKUP(B11,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>Caucasian</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -5183,8 +5737,28 @@
         <f t="shared" si="0"/>
         <v>145</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="str">
+        <f>VLOOKUP(B12,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>9% of people have chosen this contestant</v>
+      </c>
+      <c r="I12">
+        <f>VLOOKUP(B12,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="J12" t="str">
+        <f>VLOOKUP(B12,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Business Owner</v>
+      </c>
+      <c r="K12" t="str">
+        <f>VLOOKUP(B12,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'3"</v>
+      </c>
+      <c r="L12" t="str">
+        <f>VLOOKUP(B12,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>Caucasian</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -5211,8 +5785,28 @@
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="str">
+        <f>VLOOKUP(B13,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>7% of people have chosen this contestant</v>
+      </c>
+      <c r="I13">
+        <f>VLOOKUP(B13,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="J13" t="str">
+        <f>VLOOKUP(B13,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Personal Trainer</v>
+      </c>
+      <c r="K13" t="str">
+        <f>VLOOKUP(B13,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'2"</v>
+      </c>
+      <c r="L13" t="str">
+        <f>VLOOKUP(B13,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -5239,8 +5833,28 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="str">
+        <f>VLOOKUP(B14,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>2% of people have chosen this contestant</v>
+      </c>
+      <c r="I14">
+        <f>VLOOKUP(B14,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="J14" t="str">
+        <f>VLOOKUP(B14,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Attorney</v>
+      </c>
+      <c r="K14" t="str">
+        <f>VLOOKUP(B14,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>5'11"</v>
+      </c>
+      <c r="L14" t="str">
+        <f>VLOOKUP(B14,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>Caucasian</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -5267,8 +5881,28 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="str">
+        <f>VLOOKUP(B15,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>11% of people have chosen this contestant</v>
+      </c>
+      <c r="I15">
+        <f>VLOOKUP(B15,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="J15" t="str">
+        <f>VLOOKUP(B15,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Chiropractor</v>
+      </c>
+      <c r="K15" t="str">
+        <f>VLOOKUP(B15,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'2"</v>
+      </c>
+      <c r="L15" t="str">
+        <f>VLOOKUP(B15,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>Caucasian</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -5295,8 +5929,28 @@
         <f t="shared" si="0"/>
         <v>145</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="str">
+        <f>VLOOKUP(B16,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>9% of people have chosen this contestant</v>
+      </c>
+      <c r="I16">
+        <f>VLOOKUP(B16,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="J16" t="str">
+        <f>VLOOKUP(B16,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Business Owner</v>
+      </c>
+      <c r="K16" t="str">
+        <f>VLOOKUP(B16,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'3"</v>
+      </c>
+      <c r="L16" t="str">
+        <f>VLOOKUP(B16,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>Caucasian</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -5323,8 +5977,28 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="str">
+        <f>VLOOKUP(B17,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>11% of people have chosen this contestant</v>
+      </c>
+      <c r="I17">
+        <f>VLOOKUP(B17,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="J17" t="str">
+        <f>VLOOKUP(B17,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Executive Recruiter</v>
+      </c>
+      <c r="K17" t="str">
+        <f>VLOOKUP(B17,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'4"</v>
+      </c>
+      <c r="L17" t="str">
+        <f>VLOOKUP(B17,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -5351,17 +6025,37 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="str">
+        <f>VLOOKUP(B18,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>2% of people have chosen this contestant</v>
+      </c>
+      <c r="I18">
+        <f>VLOOKUP(B18,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="J18" t="str">
+        <f>VLOOKUP(B18,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Prosecuting Attorney</v>
+      </c>
+      <c r="K18" t="str">
+        <f>VLOOKUP(B18,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'3"</v>
+      </c>
+      <c r="L18" t="str">
+        <f>VLOOKUP(B18,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C19" t="str">
         <f>VLOOKUP(B19,'Contestant Points'!$A$2:$B$32,2,FALSE)</f>
-        <v>Eliminated</v>
+        <v>Still In</v>
       </c>
       <c r="D19">
         <f>VLOOKUP(B19,'Contestant Points'!$A$2:$Q$32,17,FALSE)</f>
@@ -5369,18 +6063,38 @@
       </c>
       <c r="E19">
         <f>VLOOKUP(B19,'Contestant Points'!$A$2:$R$32,18,FALSE)</f>
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="F19">
         <f>VLOOKUP(B19,'Contestant Points'!$A$2:$S$32,19,FALSE)</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="H19" t="str">
+        <f>VLOOKUP(B19,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>7% of people have chosen this contestant</v>
+      </c>
+      <c r="I19">
+        <f>VLOOKUP(B19,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="J19" t="str">
+        <f>VLOOKUP(B19,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Professional Wrestler</v>
+      </c>
+      <c r="K19" t="str">
+        <f>VLOOKUP(B19,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'</v>
+      </c>
+      <c r="L19" t="str">
+        <f>VLOOKUP(B19,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -5407,8 +6121,28 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="str">
+        <f>VLOOKUP(B20,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>2% of people have chosen this contestant</v>
+      </c>
+      <c r="I20">
+        <f>VLOOKUP(B20,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="J20" t="str">
+        <f>VLOOKUP(B20,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Attorney</v>
+      </c>
+      <c r="K20" t="str">
+        <f>VLOOKUP(B20,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>5'11"</v>
+      </c>
+      <c r="L20" t="str">
+        <f>VLOOKUP(B20,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>Caucasian</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -5434,6 +6168,26 @@
       <c r="G21">
         <f t="shared" si="0"/>
         <v>120</v>
+      </c>
+      <c r="H21" t="str">
+        <f>VLOOKUP(B21,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
+        <v>11% of people have chosen this contestant</v>
+      </c>
+      <c r="I21">
+        <f>VLOOKUP(B21,'Contestant Points'!$A$2:$D$32,4,FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="J21" t="str">
+        <f>VLOOKUP(B21,'Contestant Points'!$A$2:$E$32,5,FALSE)</f>
+        <v>Executive Recruiter</v>
+      </c>
+      <c r="K21" t="str">
+        <f>VLOOKUP(B21,'Contestant Points'!$A$2:$F$32,6,FALSE)</f>
+        <v>6'4"</v>
+      </c>
+      <c r="L21" t="str">
+        <f>VLOOKUP(B21,'Contestant Points'!$A$2:$G$32,7,FALSE)</f>
+        <v>African American</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Week 6 Stat Corrections
</commit_message>
<xml_diff>
--- a/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
+++ b/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,11 +900,11 @@
         <v>35</v>
       </c>
       <c r="V2">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="W2">
         <f>SUM(Q2:V2)</f>
-        <v>280</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -978,11 +978,11 @@
         <v>45</v>
       </c>
       <c r="V3">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="W3">
         <f t="shared" ref="W3:W32" si="6">SUM(Q3:V3)</f>
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -1368,11 +1368,11 @@
         <v>110</v>
       </c>
       <c r="V8">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
-        <v>365</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
@@ -1524,11 +1524,11 @@
         <v>10</v>
       </c>
       <c r="V10">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="W10">
         <f t="shared" si="6"/>
-        <v>390</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
@@ -1758,11 +1758,11 @@
         <v>45</v>
       </c>
       <c r="V13">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="W13">
         <f t="shared" si="6"/>
-        <v>335</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -2460,11 +2460,11 @@
         <v>115</v>
       </c>
       <c r="V22">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="W22">
         <f t="shared" si="6"/>
-        <v>450</v>
+        <v>495</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
@@ -2616,11 +2616,11 @@
         <v>85</v>
       </c>
       <c r="V24">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="W24">
         <f t="shared" si="6"/>
-        <v>345</v>
+        <v>365</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
@@ -2772,11 +2772,11 @@
         <v>40</v>
       </c>
       <c r="V26">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="W26">
         <f t="shared" si="6"/>
-        <v>235</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
@@ -3084,11 +3084,11 @@
         <v>50</v>
       </c>
       <c r="V30">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="W30">
         <f t="shared" si="6"/>
-        <v>355</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
@@ -3240,11 +3240,11 @@
         <v>80</v>
       </c>
       <c r="V32">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="W32">
         <f t="shared" si="6"/>
-        <v>265</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -3589,11 +3589,11 @@
       </c>
       <c r="I6">
         <f>VLOOKUP(B6,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K6" t="str">
         <f>VLOOKUP(B6,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -3709,11 +3709,11 @@
       </c>
       <c r="I8">
         <f>VLOOKUP(B8,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="K8" t="str">
         <f>VLOOKUP(B8,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -3769,11 +3769,11 @@
       </c>
       <c r="I9">
         <f>VLOOKUP(B9,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="K9" t="str">
         <f>VLOOKUP(B9,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -3949,11 +3949,11 @@
       </c>
       <c r="I12">
         <f>VLOOKUP(B12,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" si="0"/>
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="K12" t="str">
         <f>VLOOKUP(B12,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4069,11 +4069,11 @@
       </c>
       <c r="I14">
         <f>VLOOKUP(B14,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="K14" t="str">
         <f>VLOOKUP(B14,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4129,11 +4129,11 @@
       </c>
       <c r="I15">
         <f>VLOOKUP(B15,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K15" t="str">
         <f>VLOOKUP(B15,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4189,11 +4189,11 @@
       </c>
       <c r="I16">
         <f>VLOOKUP(B16,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>495</v>
       </c>
       <c r="K16" t="str">
         <f>VLOOKUP(B16,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4309,11 +4309,11 @@
       </c>
       <c r="I18">
         <f>VLOOKUP(B18,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>495</v>
       </c>
       <c r="K18" t="str">
         <f>VLOOKUP(B18,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4489,11 +4489,11 @@
       </c>
       <c r="I21">
         <f>VLOOKUP(B21,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="K21" t="str">
         <f>VLOOKUP(B21,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4609,11 +4609,11 @@
       </c>
       <c r="I23">
         <f>VLOOKUP(B23,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K23" t="str">
         <f>VLOOKUP(B23,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4729,11 +4729,11 @@
       </c>
       <c r="I25">
         <f>VLOOKUP(B25,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" si="0"/>
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="K25" t="str">
         <f>VLOOKUP(B25,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4849,11 +4849,11 @@
       </c>
       <c r="I27">
         <f>VLOOKUP(B27,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K27" t="str">
         <f>VLOOKUP(B27,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4909,11 +4909,11 @@
       </c>
       <c r="I28">
         <f>VLOOKUP(B28,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="K28" t="str">
         <f>VLOOKUP(B28,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -4969,11 +4969,11 @@
       </c>
       <c r="I29">
         <f>VLOOKUP(B29,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="K29" t="str">
         <f>VLOOKUP(B29,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -5029,11 +5029,11 @@
       </c>
       <c r="I30">
         <f>VLOOKUP(B30,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" si="0"/>
-        <v>390</v>
+        <v>415</v>
       </c>
       <c r="K30" t="str">
         <f>VLOOKUP(B30,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -5269,11 +5269,11 @@
       </c>
       <c r="I34">
         <f>VLOOKUP(B34,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="J34" s="3">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="K34" t="str">
         <f>VLOOKUP(B34,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -5389,11 +5389,11 @@
       </c>
       <c r="I36">
         <f>VLOOKUP(B36,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J36" s="3">
         <f t="shared" si="0"/>
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="K36" t="str">
         <f>VLOOKUP(B36,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -5749,11 +5749,11 @@
       </c>
       <c r="I42">
         <f>VLOOKUP(B42,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J42" s="3">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K42" t="str">
         <f>VLOOKUP(B42,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -5809,11 +5809,11 @@
       </c>
       <c r="I43">
         <f>VLOOKUP(B43,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="J43" s="3">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="K43" t="str">
         <f>VLOOKUP(B43,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -5929,11 +5929,11 @@
       </c>
       <c r="I45">
         <f>VLOOKUP(B45,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="J45" s="3">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>495</v>
       </c>
       <c r="K45" t="str">
         <f>VLOOKUP(B45,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -5989,11 +5989,11 @@
       </c>
       <c r="I46">
         <f>VLOOKUP(B46,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="J46" s="3">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="K46" t="str">
         <f>VLOOKUP(B46,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -6418,11 +6418,11 @@
       </c>
       <c r="I7">
         <f>VLOOKUP(B7,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K7" t="str">
         <f>VLOOKUP(B7,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -6658,11 +6658,11 @@
       </c>
       <c r="I11">
         <f>VLOOKUP(B11,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K11" t="str">
         <f>VLOOKUP(B11,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -6718,11 +6718,11 @@
       </c>
       <c r="I12">
         <f>VLOOKUP(B12,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="K12" t="str">
         <f>VLOOKUP(B12,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -6778,11 +6778,11 @@
       </c>
       <c r="I13">
         <f>VLOOKUP(B13,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="K13" t="str">
         <f>VLOOKUP(B13,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -6898,11 +6898,11 @@
       </c>
       <c r="I15">
         <f>VLOOKUP(B15,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K15" t="str">
         <f>VLOOKUP(B15,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -6958,11 +6958,11 @@
       </c>
       <c r="I16">
         <f>VLOOKUP(B16,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="K16" t="str">
         <f>VLOOKUP(B16,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -7138,11 +7138,11 @@
       </c>
       <c r="I19">
         <f>VLOOKUP(B19,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>495</v>
       </c>
       <c r="K19" t="str">
         <f>VLOOKUP(B19,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -7504,11 +7504,11 @@
       </c>
       <c r="I4">
         <f>VLOOKUP(B4,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="K4" t="str">
         <f>VLOOKUP(B4,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -7744,11 +7744,11 @@
       </c>
       <c r="I8">
         <f>VLOOKUP(B8,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="K8" t="str">
         <f>VLOOKUP(B8,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -7864,11 +7864,11 @@
       </c>
       <c r="I10">
         <f>VLOOKUP(B10,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="K10" t="str">
         <f>VLOOKUP(B10,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -7924,11 +7924,11 @@
       </c>
       <c r="I11">
         <f>VLOOKUP(B11,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>495</v>
       </c>
       <c r="K11" t="str">
         <f>VLOOKUP(B11,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -8044,11 +8044,11 @@
       </c>
       <c r="I13">
         <f>VLOOKUP(B13,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>390</v>
+        <v>415</v>
       </c>
       <c r="K13" t="str">
         <f>VLOOKUP(B13,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -8224,11 +8224,11 @@
       </c>
       <c r="I16">
         <f>VLOOKUP(B16,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>340</v>
       </c>
       <c r="K16" t="str">
         <f>VLOOKUP(B16,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -8284,11 +8284,11 @@
       </c>
       <c r="I17">
         <f>VLOOKUP(B17,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K17" t="str">
         <f>VLOOKUP(B17,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -8404,11 +8404,11 @@
       </c>
       <c r="I19">
         <f>VLOOKUP(B19,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="K19" t="str">
         <f>VLOOKUP(B19,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -8944,11 +8944,11 @@
       </c>
       <c r="I28">
         <f>VLOOKUP(B28,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K28" t="str">
         <f>VLOOKUP(B28,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -9124,11 +9124,11 @@
       </c>
       <c r="I31">
         <f>VLOOKUP(B31,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="K31" t="str">
         <f>VLOOKUP(B31,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -9244,11 +9244,11 @@
       </c>
       <c r="I33">
         <f>VLOOKUP(B33,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="K33" t="str">
         <f>VLOOKUP(B33,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -9604,11 +9604,11 @@
       </c>
       <c r="I39">
         <f>VLOOKUP(B39,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="K39" t="str">
         <f>VLOOKUP(B39,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -9664,11 +9664,11 @@
       </c>
       <c r="I40">
         <f>VLOOKUP(B40,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K40" t="str">
         <f>VLOOKUP(B40,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -9964,11 +9964,11 @@
       </c>
       <c r="I45">
         <f>VLOOKUP(B45,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K45" t="str">
         <f>VLOOKUP(B45,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -10084,11 +10084,11 @@
       </c>
       <c r="I47">
         <f>VLOOKUP(B47,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>390</v>
+        <v>415</v>
       </c>
       <c r="K47" t="str">
         <f>VLOOKUP(B47,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -10264,11 +10264,11 @@
       </c>
       <c r="I50">
         <f>VLOOKUP(B50,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="K50" t="str">
         <f>VLOOKUP(B50,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -10324,11 +10324,11 @@
       </c>
       <c r="I51">
         <f>VLOOKUP(B51,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="K51" t="str">
         <f>VLOOKUP(B51,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -10444,11 +10444,11 @@
       </c>
       <c r="I53">
         <f>VLOOKUP(B53,'Contestant Points'!$A$2:$V$32,22,FALSE)</f>
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="K53" t="str">
         <f>VLOOKUP(B53,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>

</xml_diff>

<commit_message>
Week 7 Stat Corrections
</commit_message>
<xml_diff>
--- a/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
+++ b/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Contestant Points" sheetId="4" r:id="rId1"/>
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -909,11 +909,11 @@
         <v>145</v>
       </c>
       <c r="W2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="X2">
-        <f>SUM(Q2:W2)</f>
-        <v>390</v>
+        <f t="shared" ref="X2:X32" si="0">SUM(Q2:W2)</f>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -942,33 +942,33 @@
         <v>1</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I32" si="0">H3/SUM($H$2:$H$32)</f>
+        <f t="shared" ref="I3:I32" si="1">H3/SUM($H$2:$H$32)</f>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J32" si="1">CONCATENATE(ROUND(I3*100,0),"% of people have chosen this contestant")</f>
+        <f t="shared" ref="J3:J32" si="2">CONCATENATE(ROUND(I3*100,0),"% of people have chosen this contestant")</f>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" ref="L3:L32" si="2">K3/SUM($K$2:$K$32)</f>
+        <f t="shared" ref="L3:L32" si="3">K3/SUM($K$2:$K$32)</f>
         <v>0</v>
       </c>
       <c r="M3" s="2" t="str">
-        <f t="shared" ref="M3:M32" si="3">CONCATENATE(ROUND(L3*100,0),"% of people have chosen this contestant")</f>
+        <f t="shared" ref="M3:M32" si="4">CONCATENATE(ROUND(L3*100,0),"% of people have chosen this contestant")</f>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" s="2">
-        <f t="shared" ref="O3:O32" si="4">N3/SUM($N$2:$N$32)</f>
+        <f t="shared" ref="O3:O32" si="5">N3/SUM($N$2:$N$32)</f>
         <v>0.02</v>
       </c>
       <c r="P3" s="2" t="str">
-        <f t="shared" ref="P3:P32" si="5">CONCATENATE(ROUND(O3*100,0),"% of people have chosen this contestant")</f>
+        <f t="shared" ref="P3:P32" si="6">CONCATENATE(ROUND(O3*100,0),"% of people have chosen this contestant")</f>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q3">
@@ -993,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="X3">
-        <f>SUM(Q3:W3)</f>
+        <f t="shared" si="0"/>
         <v>290</v>
       </c>
     </row>
@@ -1023,33 +1023,33 @@
         <v>3</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="J4" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7% of people have chosen this contestant</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="M4" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10% of people have chosen this contestant</v>
       </c>
       <c r="N4">
         <v>2</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P4" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q4">
@@ -1074,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="X4">
-        <f>SUM(Q4:W4)</f>
+        <f t="shared" si="0"/>
         <v>190</v>
       </c>
     </row>
@@ -1104,33 +1104,33 @@
         <v>0</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J5" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M5" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P5" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q5">
@@ -1155,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="X5">
-        <f>SUM(Q5:W5)</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
@@ -1185,33 +1185,33 @@
         <v>2</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M6" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N6">
         <v>6</v>
       </c>
       <c r="O6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12</v>
       </c>
       <c r="P6" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12% of people have chosen this contestant</v>
       </c>
       <c r="Q6">
@@ -1236,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="X6">
-        <f>SUM(Q6:W6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1266,33 +1266,33 @@
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J7" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M7" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q7">
@@ -1317,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="X7">
-        <f>SUM(Q7:W7)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -1347,33 +1347,33 @@
         <v>5</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="J8" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11% of people have chosen this contestant</v>
       </c>
       <c r="K8">
         <v>3</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="M8" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15% of people have chosen this contestant</v>
       </c>
       <c r="N8">
         <v>4</v>
       </c>
       <c r="O8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.08</v>
       </c>
       <c r="P8" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8% of people have chosen this contestant</v>
       </c>
       <c r="Q8">
@@ -1398,7 +1398,7 @@
         <v>80</v>
       </c>
       <c r="X8">
-        <f>SUM(Q8:W8)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
     </row>
@@ -1428,33 +1428,33 @@
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J9" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M9" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="P9" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q9">
@@ -1479,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="X9">
-        <f>SUM(Q9:W9)</f>
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
@@ -1509,33 +1509,33 @@
         <v>1</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J10" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M10" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N10">
         <v>2</v>
       </c>
       <c r="O10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P10" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q10">
@@ -1560,7 +1560,7 @@
         <v>90</v>
       </c>
       <c r="X10">
-        <f>SUM(Q10:W10)</f>
+        <f t="shared" si="0"/>
         <v>505</v>
       </c>
     </row>
@@ -1590,33 +1590,33 @@
         <v>5</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="J11" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11% of people have chosen this contestant</v>
       </c>
       <c r="K11">
         <v>3</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
       <c r="M11" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15% of people have chosen this contestant</v>
       </c>
       <c r="N11">
         <v>7</v>
       </c>
       <c r="O11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="P11" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14% of people have chosen this contestant</v>
       </c>
       <c r="Q11">
@@ -1641,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="X11">
-        <f>SUM(Q11:W11)</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
@@ -1671,33 +1671,33 @@
         <v>6</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13333333333333333</v>
       </c>
       <c r="J12" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13% of people have chosen this contestant</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="M12" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5% of people have chosen this contestant</v>
       </c>
       <c r="N12">
         <v>2</v>
       </c>
       <c r="O12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P12" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q12">
@@ -1722,7 +1722,7 @@
         <v>0</v>
       </c>
       <c r="X12">
-        <f>SUM(Q12:W12)</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
@@ -1752,33 +1752,33 @@
         <v>3</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="J13" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7% of people have chosen this contestant</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="M13" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5% of people have chosen this contestant</v>
       </c>
       <c r="N13">
         <v>2</v>
       </c>
       <c r="O13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P13" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q13">
@@ -1803,7 +1803,7 @@
         <v>75</v>
       </c>
       <c r="X13">
-        <f>SUM(Q13:W13)</f>
+        <f t="shared" si="0"/>
         <v>440</v>
       </c>
     </row>
@@ -1833,33 +1833,33 @@
         <v>0</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J14" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="M14" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5% of people have chosen this contestant</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="P14" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q14">
@@ -1884,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="X14">
-        <f>SUM(Q14:W14)</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
@@ -1914,33 +1914,33 @@
         <v>0</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J15" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M15" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P15" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q15">
@@ -1965,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="X15">
-        <f>SUM(Q15:W15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1995,33 +1995,33 @@
         <v>0</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J16" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M16" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P16" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q16">
@@ -2046,7 +2046,7 @@
         <v>0</v>
       </c>
       <c r="X16">
-        <f>SUM(Q16:W16)</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
@@ -2076,33 +2076,33 @@
         <v>1</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K17">
         <v>4</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
       <c r="M17" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20% of people have chosen this contestant</v>
       </c>
       <c r="N17">
         <v>3</v>
       </c>
       <c r="O17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P17" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q17">
@@ -2127,7 +2127,7 @@
         <v>0</v>
       </c>
       <c r="X17">
-        <f>SUM(Q17:W17)</f>
+        <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
@@ -2157,33 +2157,33 @@
         <v>1</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M18" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N18">
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P18" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q18">
@@ -2208,7 +2208,7 @@
         <v>0</v>
       </c>
       <c r="X18">
-        <f>SUM(Q18:W18)</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
@@ -2238,33 +2238,33 @@
         <v>1</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M19" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N19">
         <v>3</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P19" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q19">
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="X19">
-        <f>SUM(Q19:W19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2319,33 +2319,33 @@
         <v>0</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J20" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M20" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P20" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q20">
@@ -2370,7 +2370,7 @@
         <v>0</v>
       </c>
       <c r="X20">
-        <f>SUM(Q20:W20)</f>
+        <f t="shared" si="0"/>
         <v>145</v>
       </c>
     </row>
@@ -2400,33 +2400,33 @@
         <v>1</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J21" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K21">
         <v>2</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="M21" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10% of people have chosen this contestant</v>
       </c>
       <c r="N21">
         <v>2</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P21" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q21">
@@ -2451,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="X21">
-        <f>SUM(Q21:W21)</f>
+        <f t="shared" si="0"/>
         <v>205</v>
       </c>
     </row>
@@ -2481,33 +2481,33 @@
         <v>3</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="J22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7% of people have chosen this contestant</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="M22" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5% of people have chosen this contestant</v>
       </c>
       <c r="N22">
         <v>1</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="P22" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q22">
@@ -2532,7 +2532,7 @@
         <v>0</v>
       </c>
       <c r="X22">
-        <f>SUM(Q22:W22)</f>
+        <f t="shared" si="0"/>
         <v>495</v>
       </c>
     </row>
@@ -2562,33 +2562,33 @@
         <v>1</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M23" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
       <c r="O23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P23" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q23">
@@ -2613,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="X23">
-        <f>SUM(Q23:W23)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2643,33 +2643,33 @@
         <v>1</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M24" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N24">
         <v>0</v>
       </c>
       <c r="O24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P24" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q24">
@@ -2694,7 +2694,7 @@
         <v>0</v>
       </c>
       <c r="X24">
-        <f>SUM(Q24:W24)</f>
+        <f t="shared" si="0"/>
         <v>365</v>
       </c>
     </row>
@@ -2724,33 +2724,33 @@
         <v>0</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J25" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M25" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P25" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q25">
@@ -2775,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="X25">
-        <f>SUM(Q25:W25)</f>
+        <f t="shared" si="0"/>
         <v>135</v>
       </c>
     </row>
@@ -2805,33 +2805,33 @@
         <v>1</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J26" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M26" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N26">
         <v>2</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
       <c r="P26" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="Q26">
@@ -2856,7 +2856,7 @@
         <v>30</v>
       </c>
       <c r="X26">
-        <f>SUM(Q26:W26)</f>
+        <f t="shared" si="0"/>
         <v>285</v>
       </c>
     </row>
@@ -2886,33 +2886,33 @@
         <v>2</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="J27" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M27" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N27">
         <v>3</v>
       </c>
       <c r="O27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P27" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q27">
@@ -2937,7 +2937,7 @@
         <v>0</v>
       </c>
       <c r="X27">
-        <f>SUM(Q27:W27)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -2967,33 +2967,33 @@
         <v>0</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J28" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M28" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N28">
         <v>0</v>
       </c>
       <c r="O28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P28" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q28">
@@ -3018,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="X28">
-        <f>SUM(Q28:W28)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -3048,33 +3048,33 @@
         <v>1</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2222222222222223E-2</v>
       </c>
       <c r="J29" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M29" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N29">
         <v>0</v>
       </c>
       <c r="O29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P29" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="Q29">
@@ -3099,7 +3099,7 @@
         <v>0</v>
       </c>
       <c r="X29">
-        <f>SUM(Q29:W29)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -3129,33 +3129,33 @@
         <v>4</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.8888888888888892E-2</v>
       </c>
       <c r="J30" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9% of people have chosen this contestant</v>
       </c>
       <c r="K30">
         <v>2</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="M30" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10% of people have chosen this contestant</v>
       </c>
       <c r="N30">
         <v>1</v>
       </c>
       <c r="O30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="P30" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2% of people have chosen this contestant</v>
       </c>
       <c r="Q30">
@@ -3180,7 +3180,7 @@
         <v>90</v>
       </c>
       <c r="X30">
-        <f>SUM(Q30:W30)</f>
+        <f t="shared" si="0"/>
         <v>465</v>
       </c>
     </row>
@@ -3210,33 +3210,33 @@
         <v>0</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J31" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="K31">
         <v>0</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M31" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N31">
         <v>3</v>
       </c>
       <c r="O31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P31" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q31">
@@ -3261,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="X31">
-        <f>SUM(Q31:W31)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -3291,33 +3291,33 @@
         <v>2</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.4444444444444446E-2</v>
       </c>
       <c r="J32" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4% of people have chosen this contestant</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M32" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0% of people have chosen this contestant</v>
       </c>
       <c r="N32">
         <v>3</v>
       </c>
       <c r="O32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="P32" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6% of people have chosen this contestant</v>
       </c>
       <c r="Q32">
@@ -3342,7 +3342,7 @@
         <v>0</v>
       </c>
       <c r="X32">
-        <f>SUM(Q32:W32)</f>
+        <f t="shared" si="0"/>
         <v>275</v>
       </c>
     </row>
@@ -3355,9 +3355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="L55" sqref="L55"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8181,9 +8179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9176,11 +9172,11 @@
       </c>
       <c r="J16">
         <f>VLOOKUP(B16,'Contestant Points'!$A$2:$W$32,23,FALSE)</f>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="L16" t="str">
         <f>VLOOKUP(B16,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>

</xml_diff>

<commit_message>
Week 10 Stat Correction
</commit_message>
<xml_diff>
--- a/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
+++ b/2017 Bachelorette Fantasy/BacheloretteFantasy2017.xlsx
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1972,11 +1972,11 @@
         <v>5</v>
       </c>
       <c r="AA13">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="AB13">
         <f t="shared" si="6"/>
-        <v>700</v>
+        <v>790</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
@@ -4443,11 +4443,11 @@
       </c>
       <c r="N9">
         <f>VLOOKUP(B9,'Contestant Points'!$A$2:$AA$32,27,FALSE)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>790</v>
       </c>
       <c r="P9" t="str">
         <f>VLOOKUP(B9,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -6043,11 +6043,11 @@
       </c>
       <c r="N29">
         <f>VLOOKUP(B29,'Contestant Points'!$A$2:$AA$32,27,FALSE)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O29" s="3">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>790</v>
       </c>
       <c r="P29" t="str">
         <f>VLOOKUP(B29,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -7163,11 +7163,11 @@
       </c>
       <c r="N43">
         <f>VLOOKUP(B43,'Contestant Points'!$A$2:$AA$32,27,FALSE)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O43" s="3">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>790</v>
       </c>
       <c r="P43" t="str">
         <f>VLOOKUP(B43,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -7551,11 +7551,11 @@
       </c>
       <c r="N48">
         <f>VLOOKUP(B48,'Contestant Points'!$A$2:$AA$32,27,FALSE)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O48" s="3">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>425</v>
       </c>
       <c r="P48" t="str">
         <f>VLOOKUP(B48,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -9111,11 +9111,11 @@
       </c>
       <c r="N13">
         <f>VLOOKUP(B13,'Contestant Points'!$A$2:$AA$32,27,FALSE)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>790</v>
       </c>
       <c r="P13" t="str">
         <f>VLOOKUP(B13,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -10074,11 +10074,11 @@
       </c>
       <c r="N4">
         <f>VLOOKUP(B4,'Contestant Points'!$A$2:$AA$32,27,FALSE)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>790</v>
       </c>
       <c r="P4" t="str">
         <f>VLOOKUP(B4,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -10394,11 +10394,11 @@
       </c>
       <c r="N8">
         <f>VLOOKUP(B8,'Contestant Points'!$A$2:$AA$32,27,FALSE)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>790</v>
       </c>
       <c r="P8" t="str">
         <f>VLOOKUP(B8,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>
@@ -14604,11 +14604,11 @@
       </c>
       <c r="N61">
         <f>VLOOKUP(B61,'Contestant Points'!$A$2:$AA$32,27,FALSE)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="O61">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>425</v>
       </c>
       <c r="P61" t="str">
         <f>VLOOKUP(B61,'Contestant Points'!$A$2:$J$32,10,FALSE)</f>

</xml_diff>